<commit_message>
FInd Empty Coulmn Automatically
</commit_message>
<xml_diff>
--- a/Attendance_Data.xlsx
+++ b/Attendance_Data.xlsx
@@ -673,14 +673,30 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Absent</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -733,14 +749,34 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>Absent</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -796,11 +832,27 @@
           <t>Absent</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
@@ -853,14 +905,30 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>Absent</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
@@ -913,14 +981,26 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Absent</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>

</xml_diff>